<commit_message>
Added features: range of values user selection and x-axis date format user specification.
</commit_message>
<xml_diff>
--- a/public/DummyData.xlsx
+++ b/public/DummyData.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\working\waccache\MI1PEPF000001A2\EXCELCNV\de0529d3-6cd0-4ffc-b8f9-aa01a730b96f\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="46" documentId="8_{F1FE87A4-FDF6-4ABF-B5EC-2D56D29411FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{57294F4A-63CD-4FA5-9774-7833935C5CE1}"/>
+  <xr:revisionPtr revIDLastSave="89" documentId="8_{F1FE87A4-FDF6-4ABF-B5EC-2D56D29411FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B3DA4827-7DFB-4A7E-AAF5-AC1417DACB64}"/>
   <bookViews>
     <workbookView xWindow="-60" yWindow="-60" windowWidth="15480" windowHeight="11640" xr2:uid="{28DE5DFB-25A8-47E3-BC07-85B5F3805695}"/>
   </bookViews>
   <sheets>
     <sheet name="xaxis-date" sheetId="1" r:id="rId1"/>
     <sheet name="xaxis-num" sheetId="2" r:id="rId2"/>
+    <sheet name="xaxis-cat" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -37,9 +38,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
   <si>
-    <t>date</t>
+    <t>Date</t>
   </si>
   <si>
     <t>avg_outflow</t>
@@ -93,13 +94,121 @@
     <t>VG</t>
   </si>
   <si>
-    <t>x</t>
+    <t>Number</t>
   </si>
   <si>
-    <t>sin(x)</t>
+    <t>sin</t>
   </si>
   <si>
-    <t>cos(x)</t>
+    <t>cos</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Car sales 2019</t>
+  </si>
+  <si>
+    <t>Car sales 2020</t>
+  </si>
+  <si>
+    <t>Car sales 2021</t>
+  </si>
+  <si>
+    <t>Car sales 2022</t>
+  </si>
+  <si>
+    <t>Car sales 2023</t>
+  </si>
+  <si>
+    <t>Toyota</t>
+  </si>
+  <si>
+    <t>Volkswagen</t>
+  </si>
+  <si>
+    <t>Honda</t>
+  </si>
+  <si>
+    <t>Ford</t>
+  </si>
+  <si>
+    <t>Hyundai</t>
+  </si>
+  <si>
+    <t>Nissan</t>
+  </si>
+  <si>
+    <t>Suzuki</t>
+  </si>
+  <si>
+    <t>Kia</t>
+  </si>
+  <si>
+    <t>Chevrolet</t>
+  </si>
+  <si>
+    <t>BYD</t>
+  </si>
+  <si>
+    <t>BMW</t>
+  </si>
+  <si>
+    <t>Mercedes-Benz</t>
+  </si>
+  <si>
+    <t>Audi</t>
+  </si>
+  <si>
+    <t>Tesla</t>
+  </si>
+  <si>
+    <t>Renault</t>
+  </si>
+  <si>
+    <t>Fiat</t>
+  </si>
+  <si>
+    <t>Mazda</t>
+  </si>
+  <si>
+    <t>Peugeot</t>
+  </si>
+  <si>
+    <t>Changan</t>
+  </si>
+  <si>
+    <t>Jeep</t>
+  </si>
+  <si>
+    <t>Geely</t>
+  </si>
+  <si>
+    <t>Tata</t>
+  </si>
+  <si>
+    <t>Subaru</t>
+  </si>
+  <si>
+    <t>Wuling</t>
+  </si>
+  <si>
+    <t>GAC</t>
+  </si>
+  <si>
+    <t>Skoda</t>
+  </si>
+  <si>
+    <t>Chery</t>
+  </si>
+  <si>
+    <t>Daihatsu</t>
+  </si>
+  <si>
+    <t>Volvo</t>
+  </si>
+  <si>
+    <t>Buick</t>
   </si>
 </sst>
 </file>
@@ -586,10 +695,14 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -959,58 +1072,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Q1" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="R1" s="6" t="s">
         <v>17</v>
       </c>
     </row>
@@ -79802,13 +79915,13 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" t="s">
+      <c r="A1" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="6" t="s">
         <v>20</v>
       </c>
     </row>
@@ -87618,4 +87731,639 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBF1E688-0F13-4BE2-81DB-26D6FFACCF8C}">
+  <dimension ref="A1:F31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="4">
+        <v>8578155</v>
+      </c>
+      <c r="C2" s="4">
+        <v>7583468</v>
+      </c>
+      <c r="D2" s="4">
+        <v>8254315</v>
+      </c>
+      <c r="E2" s="4">
+        <v>8282491</v>
+      </c>
+      <c r="F2" s="4">
+        <v>8569973</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="4">
+        <v>6669186</v>
+      </c>
+      <c r="C3" s="4">
+        <v>5552064</v>
+      </c>
+      <c r="D3" s="4">
+        <v>5080426</v>
+      </c>
+      <c r="E3" s="4">
+        <v>4807921</v>
+      </c>
+      <c r="F3" s="4">
+        <v>4965621</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="4">
+        <v>4958195</v>
+      </c>
+      <c r="C4" s="4">
+        <v>4284278</v>
+      </c>
+      <c r="D4" s="4">
+        <v>4219686</v>
+      </c>
+      <c r="E4" s="4">
+        <v>3643675</v>
+      </c>
+      <c r="F4" s="4">
+        <v>3774161</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="4">
+        <v>5016542</v>
+      </c>
+      <c r="C5" s="4">
+        <v>4048340</v>
+      </c>
+      <c r="D5" s="4">
+        <v>3751737</v>
+      </c>
+      <c r="E5" s="4">
+        <v>3529127</v>
+      </c>
+      <c r="F5" s="4">
+        <v>3729817</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="4">
+        <v>4168921</v>
+      </c>
+      <c r="C6" s="4">
+        <v>3405642</v>
+      </c>
+      <c r="D6" s="4">
+        <v>3606423</v>
+      </c>
+      <c r="E6" s="4">
+        <v>3382405</v>
+      </c>
+      <c r="F6" s="4">
+        <v>3540787</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="4">
+        <v>4497703</v>
+      </c>
+      <c r="C7" s="4">
+        <v>3533792</v>
+      </c>
+      <c r="D7" s="4">
+        <v>3449805</v>
+      </c>
+      <c r="E7" s="4">
+        <v>2824267</v>
+      </c>
+      <c r="F7" s="4">
+        <v>2975048</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="4">
+        <v>2910805</v>
+      </c>
+      <c r="C8" s="4">
+        <v>2374281</v>
+      </c>
+      <c r="D8" s="4">
+        <v>2664574</v>
+      </c>
+      <c r="E8" s="4">
+        <v>2841135</v>
+      </c>
+      <c r="F8" s="4">
+        <v>2916149</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="4">
+        <v>2667969</v>
+      </c>
+      <c r="C9" s="4">
+        <v>2571520</v>
+      </c>
+      <c r="D9" s="4">
+        <v>2771272</v>
+      </c>
+      <c r="E9" s="4">
+        <v>2687205</v>
+      </c>
+      <c r="F9" s="4">
+        <v>2731370</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" s="4">
+        <v>3890933</v>
+      </c>
+      <c r="C10" s="4">
+        <v>3187353</v>
+      </c>
+      <c r="D10" s="4">
+        <v>2522139</v>
+      </c>
+      <c r="E10" s="4">
+        <v>2518572</v>
+      </c>
+      <c r="F10" s="4">
+        <v>2692391</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="4">
+        <v>457849</v>
+      </c>
+      <c r="C11" s="4">
+        <v>404982</v>
+      </c>
+      <c r="D11" s="4">
+        <v>738285</v>
+      </c>
+      <c r="E11" s="4">
+        <v>1819983</v>
+      </c>
+      <c r="F11" s="4">
+        <v>2683743</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" s="4">
+        <v>1982974</v>
+      </c>
+      <c r="C12" s="4">
+        <v>1816967</v>
+      </c>
+      <c r="D12" s="4">
+        <v>1978307</v>
+      </c>
+      <c r="E12" s="4">
+        <v>1896148</v>
+      </c>
+      <c r="F12" s="4">
+        <v>2101487</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" s="4">
+        <v>2467238</v>
+      </c>
+      <c r="C13" s="4">
+        <v>2195013</v>
+      </c>
+      <c r="D13" s="4">
+        <v>2048876</v>
+      </c>
+      <c r="E13" s="4">
+        <v>1992876</v>
+      </c>
+      <c r="F13" s="4">
+        <v>2063820</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" s="4">
+        <v>1744566</v>
+      </c>
+      <c r="C14" s="4">
+        <v>1600355</v>
+      </c>
+      <c r="D14" s="4">
+        <v>1589605</v>
+      </c>
+      <c r="E14" s="4">
+        <v>1515751</v>
+      </c>
+      <c r="F14" s="4">
+        <v>1772892</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" s="4">
+        <v>304783</v>
+      </c>
+      <c r="C15" s="4">
+        <v>456406</v>
+      </c>
+      <c r="D15" s="4">
+        <v>1030513</v>
+      </c>
+      <c r="E15" s="4">
+        <v>1342112</v>
+      </c>
+      <c r="F15" s="4">
+        <v>1770354</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16" s="4">
+        <v>2208122</v>
+      </c>
+      <c r="C16" s="4">
+        <v>1711942</v>
+      </c>
+      <c r="D16" s="4">
+        <v>1586735</v>
+      </c>
+      <c r="E16" s="4">
+        <v>1362848</v>
+      </c>
+      <c r="F16" s="4">
+        <v>1435847</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" s="4">
+        <v>1321366</v>
+      </c>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4">
+        <v>1261296</v>
+      </c>
+      <c r="E17" s="4">
+        <v>1151327</v>
+      </c>
+      <c r="F17" s="4">
+        <v>1235442</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" s="4">
+        <v>1453621</v>
+      </c>
+      <c r="C18" s="4">
+        <v>1225875</v>
+      </c>
+      <c r="D18" s="4">
+        <v>1218746</v>
+      </c>
+      <c r="E18" s="4">
+        <v>1059059</v>
+      </c>
+      <c r="F18" s="4">
+        <v>1182034</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B19" s="4">
+        <v>1413023</v>
+      </c>
+      <c r="C19" s="4">
+        <v>28152</v>
+      </c>
+      <c r="D19" s="4">
+        <v>1161207</v>
+      </c>
+      <c r="E19" s="4">
+        <v>1012749</v>
+      </c>
+      <c r="F19" s="4">
+        <v>1060432</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B20" s="4">
+        <v>752093</v>
+      </c>
+      <c r="C20" s="4">
+        <v>842825</v>
+      </c>
+      <c r="D20" s="4">
+        <v>1011372</v>
+      </c>
+      <c r="E20" s="4">
+        <v>1112791</v>
+      </c>
+      <c r="F20" s="4">
+        <v>1011336</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B21" s="4">
+        <v>1438428</v>
+      </c>
+      <c r="C21" s="4">
+        <v>40693</v>
+      </c>
+      <c r="D21" s="4">
+        <v>1224426</v>
+      </c>
+      <c r="E21" s="4">
+        <v>1066392</v>
+      </c>
+      <c r="F21" s="4">
+        <v>1008181</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B22" s="4">
+        <v>1238846</v>
+      </c>
+      <c r="C22" s="4">
+        <v>1152860</v>
+      </c>
+      <c r="D22" s="4">
+        <v>1108311</v>
+      </c>
+      <c r="E22" s="4">
+        <v>925117</v>
+      </c>
+      <c r="F22" s="4">
+        <v>1002311</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B23" s="4">
+        <v>531261</v>
+      </c>
+      <c r="C23" s="4">
+        <v>377307</v>
+      </c>
+      <c r="D23" s="4">
+        <v>643751</v>
+      </c>
+      <c r="E23" s="4">
+        <v>994955</v>
+      </c>
+      <c r="F23" s="4">
+        <v>937087</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B24" s="4">
+        <v>1001482</v>
+      </c>
+      <c r="C24" s="4">
+        <v>849514</v>
+      </c>
+      <c r="D24" s="4">
+        <v>831345</v>
+      </c>
+      <c r="E24" s="4">
+        <v>778137</v>
+      </c>
+      <c r="F24" s="4">
+        <v>889975</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B25" s="4">
+        <v>397221</v>
+      </c>
+      <c r="C25" s="4">
+        <v>553453</v>
+      </c>
+      <c r="D25" s="4">
+        <v>1074685</v>
+      </c>
+      <c r="E25" s="4">
+        <v>871765</v>
+      </c>
+      <c r="F25" s="4">
+        <v>851935</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B26" s="4">
+        <v>388208</v>
+      </c>
+      <c r="C26" s="4">
+        <v>353882</v>
+      </c>
+      <c r="D26" s="4">
+        <v>440852</v>
+      </c>
+      <c r="E26" s="4">
+        <v>611615</v>
+      </c>
+      <c r="F26" s="4">
+        <v>839537</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B27" s="4">
+        <v>1190325</v>
+      </c>
+      <c r="C27" s="4">
+        <v>951359</v>
+      </c>
+      <c r="D27" s="4">
+        <v>816621</v>
+      </c>
+      <c r="E27" s="4">
+        <v>696725</v>
+      </c>
+      <c r="F27" s="4">
+        <v>804710</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B28" s="4">
+        <v>454869</v>
+      </c>
+      <c r="C28" s="4">
+        <v>503032</v>
+      </c>
+      <c r="D28" s="4">
+        <v>769973</v>
+      </c>
+      <c r="E28" s="4">
+        <v>729454</v>
+      </c>
+      <c r="F28" s="4">
+        <v>799063</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B29" s="4">
+        <v>837927</v>
+      </c>
+      <c r="C29" s="4">
+        <v>684712</v>
+      </c>
+      <c r="D29" s="4">
+        <v>738593</v>
+      </c>
+      <c r="E29" s="4">
+        <v>779413</v>
+      </c>
+      <c r="F29" s="4">
+        <v>783416</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B30" s="4">
+        <v>742170</v>
+      </c>
+      <c r="C30" s="4">
+        <v>712329</v>
+      </c>
+      <c r="D30" s="4">
+        <v>770727</v>
+      </c>
+      <c r="E30" s="4">
+        <v>688348</v>
+      </c>
+      <c r="F30" s="4">
+        <v>750483</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B31" s="4">
+        <v>1095745</v>
+      </c>
+      <c r="C31" s="4">
+        <v>1106686</v>
+      </c>
+      <c r="D31" s="4">
+        <v>1025650</v>
+      </c>
+      <c r="E31" s="4">
+        <v>745722</v>
+      </c>
+      <c r="F31" s="4">
+        <v>702821</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>